<commit_message>
async await in querys and mudularizated uptedate client
</commit_message>
<xml_diff>
--- a/src/ExcelDocuments/files/client.xlsx
+++ b/src/ExcelDocuments/files/client.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
   <si>
     <t>Id</t>
   </si>
@@ -37,171 +37,174 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Mariano</t>
-  </si>
-  <si>
-    <t>Jose</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>dDAS</t>
-  </si>
-  <si>
-    <t>MOVA14082123</t>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>HSFF9808KOPOIN92D2</t>
   </si>
   <si>
     <t>2021-01-27T03:33:20.000Z</t>
   </si>
   <si>
-    <t>Raul</t>
+    <t>Armando</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Mora</t>
+  </si>
+  <si>
+    <t>Valles</t>
+  </si>
+  <si>
+    <t>MOVAAAAAA92D2</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>Ramirez</t>
+  </si>
+  <si>
+    <t>Rocha</t>
+  </si>
+  <si>
+    <t>HCH1308AAA92D2</t>
+  </si>
+  <si>
+    <t>Luis</t>
   </si>
   <si>
     <t>Fernando</t>
   </si>
   <si>
-    <t>Mendias</t>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>AMVK1234UNODOSR2D2</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Enriquez</t>
+  </si>
+  <si>
+    <t>AMVKP3P2UNODOSR2D2</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>Ramos</t>
+  </si>
+  <si>
+    <t>RARFA0989HCHOIN9D2</t>
+  </si>
+  <si>
+    <t>Citlaly</t>
+  </si>
+  <si>
+    <t>Sosa</t>
+  </si>
+  <si>
+    <t>Gardea</t>
+  </si>
+  <si>
+    <t>RARFA0989HCHOID2</t>
+  </si>
+  <si>
+    <t>Zulema</t>
+  </si>
+  <si>
+    <t>RARFA0989HCHOIND27</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>Roberta</t>
+  </si>
+  <si>
+    <t>123A0989HCN9R2D</t>
+  </si>
+  <si>
+    <t>Luisa</t>
+  </si>
+  <si>
+    <t>Rojas</t>
+  </si>
+  <si>
+    <t>Valdez</t>
+  </si>
+  <si>
+    <t>HCHA0989HCN9R2D</t>
+  </si>
+  <si>
+    <t>Valeria</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>HCHA9809HCHOIN9R2D</t>
+  </si>
+  <si>
+    <t>Claudia</t>
+  </si>
+  <si>
+    <t>Monte</t>
+  </si>
+  <si>
+    <t>HCHA9809MCHOIN9R2D</t>
+  </si>
+  <si>
+    <t>Octavio</t>
+  </si>
+  <si>
+    <t>Rofolfo</t>
+  </si>
+  <si>
+    <t>guevara</t>
+  </si>
+  <si>
+    <t>Sagarnaga</t>
+  </si>
+  <si>
+    <t>HCHA909MCHOIN9R2D</t>
+  </si>
+  <si>
+    <t>Martha</t>
+  </si>
+  <si>
+    <t>Elena</t>
+  </si>
+  <si>
+    <t>Navarrete</t>
   </si>
   <si>
     <t>Gonzales</t>
   </si>
   <si>
-    <t>HSFF1408HCHOIN92D3</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Miramonetes</t>
-  </si>
-  <si>
-    <t>Garcia</t>
-  </si>
-  <si>
-    <t>HSFF9808HCHOIN92D2</t>
-  </si>
-  <si>
-    <t>Luis</t>
-  </si>
-  <si>
-    <t>Lopez</t>
-  </si>
-  <si>
-    <t>AMVK1234UNODOSR2D2</t>
-  </si>
-  <si>
-    <t>Carlos</t>
-  </si>
-  <si>
-    <t>Perez</t>
-  </si>
-  <si>
-    <t>Enriquez</t>
-  </si>
-  <si>
-    <t>Valles</t>
-  </si>
-  <si>
-    <t>AMVKP3P2UNODOSR2D2</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Rodriguez</t>
-  </si>
-  <si>
-    <t>Ramos</t>
-  </si>
-  <si>
-    <t>RARFA0989HCHOIN9D2</t>
-  </si>
-  <si>
-    <t>Citlaly</t>
-  </si>
-  <si>
-    <t>Sosa</t>
-  </si>
-  <si>
-    <t>Gardea</t>
-  </si>
-  <si>
-    <t>RARFA0989HCHOID2</t>
-  </si>
-  <si>
-    <t>Zulema</t>
-  </si>
-  <si>
-    <t>RARFA0989HCHOIND27</t>
-  </si>
-  <si>
-    <t>Andrea</t>
-  </si>
-  <si>
-    <t>Roberta</t>
-  </si>
-  <si>
-    <t>123A0989HCN9R2D</t>
-  </si>
-  <si>
-    <t>Luisa</t>
-  </si>
-  <si>
-    <t>Rojas</t>
-  </si>
-  <si>
-    <t>Valdez</t>
-  </si>
-  <si>
-    <t>HCHA0989HCN9R2D</t>
-  </si>
-  <si>
-    <t>Valeria</t>
-  </si>
-  <si>
-    <t>Sebastian</t>
-  </si>
-  <si>
-    <t>Martinez</t>
-  </si>
-  <si>
-    <t>HCHA9809HCHOIN9R2D</t>
-  </si>
-  <si>
-    <t>Claudia</t>
-  </si>
-  <si>
-    <t>Monte</t>
-  </si>
-  <si>
-    <t>HCHA9809MCHOIN9R2D</t>
-  </si>
-  <si>
-    <t>Octavio</t>
-  </si>
-  <si>
-    <t>Rofolfo</t>
-  </si>
-  <si>
-    <t>guevara</t>
-  </si>
-  <si>
-    <t>Sagarnaga</t>
-  </si>
-  <si>
-    <t>HCHA909MCHOIN9R2D</t>
-  </si>
-  <si>
-    <t>Martha</t>
-  </si>
-  <si>
-    <t>Elena</t>
-  </si>
-  <si>
-    <t>Navarrete</t>
-  </si>
-  <si>
     <t>MCHT909MCHOIN9R2D</t>
   </si>
   <si>
@@ -227,12 +230,6 @@
   </si>
   <si>
     <t>EJFF8385HCHOIN92R2</t>
-  </si>
-  <si>
-    <t>Armando</t>
-  </si>
-  <si>
-    <t>Mora</t>
   </si>
   <si>
     <t>MSDF1408HCHASE0989</t>
@@ -709,10 +706,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
@@ -738,16 +735,16 @@
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -761,19 +758,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
       </c>
       <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
         <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -787,10 +784,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -816,7 +813,7 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>36</v>
@@ -842,7 +839,7 @@
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
         <v>36</v>
@@ -868,13 +865,13 @@
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
         <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
         <v>43</v>
@@ -894,7 +891,7 @@
         <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
         <v>45</v>
@@ -926,7 +923,7 @@
         <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
         <v>51</v>
@@ -946,13 +943,13 @@
         <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
         <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
         <v>54</v>
@@ -1004,10 +1001,10 @@
         <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G15">
         <v>5</v>
@@ -1021,19 +1018,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G16">
         <v>5</v>
@@ -1047,19 +1044,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G17">
         <v>3</v>
@@ -1073,19 +1070,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
         <v>73</v>
-      </c>
-      <c r="E18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" t="s">
-        <v>74</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1099,25 +1096,25 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>